<commit_message>
fixing issues in pipenv virtual invironment
</commit_message>
<xml_diff>
--- a/endpoints.xlsx
+++ b/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Grad Proj\grad-proj-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A2D9AE-5E2D-4DDF-A43C-EAA50A7F4DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3259365-F8FB-4D50-9BFD-B99BF7C306B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="endpoints" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
   <si>
     <t>route</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>make plan to visit places</t>
-  </si>
-  <si>
-    <t>hash</t>
   </si>
   <si>
     <t>not verified</t>
@@ -337,7 +334,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +387,13 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,7 +497,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -561,7 +565,8 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -856,8 +861,8 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -952,9 +957,7 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="41" t="s">
-        <v>97</v>
-      </c>
+      <c r="H5" s="41"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1065,9 +1068,7 @@
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="41" t="s">
-        <v>97</v>
-      </c>
+      <c r="H12" s="42"/>
       <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1097,7 +1098,7 @@
         <v>403</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" s="38"/>
       <c r="I14" s="17"/>
@@ -1197,9 +1198,7 @@
       <c r="G20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="41" t="s">
-        <v>97</v>
-      </c>
+      <c r="H20" s="42"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1812,7 +1811,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>51</v>
@@ -1955,7 +1954,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>51</v>
@@ -2351,9 +2350,7 @@
       <c r="G94" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H94" s="41" t="s">
-        <v>97</v>
-      </c>
+      <c r="H94" s="42"/>
       <c r="I94" s="17"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -2384,7 +2381,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>

</xml_diff>

<commit_message>
adding endpoints placeholders for places blueprint
</commit_message>
<xml_diff>
--- a/endpoints.xlsx
+++ b/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Grad Proj\grad-proj-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45685789-8C8F-4C03-AB34-30F1AD3DC918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBBD655-CB88-4C75-A139-65E18B1E89AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="endpoints" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
   <si>
     <t>route</t>
   </si>
@@ -48,9 +48,6 @@
     <t>auth/signup</t>
   </si>
   <si>
-    <t>post</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>places/rec</t>
   </si>
   <si>
-    <t>get</t>
-  </si>
-  <si>
     <t>Authorization</t>
   </si>
   <si>
@@ -120,12 +114,6 @@
     <t>rating</t>
   </si>
   <si>
-    <t>places/search</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -180,9 +168,6 @@
     <t>added</t>
   </si>
   <si>
-    <t>delete</t>
-  </si>
-  <si>
     <t>delete place from favorites</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
     <t>comments/&lt;id&gt;</t>
   </si>
   <si>
-    <t>put</t>
-  </si>
-  <si>
     <t>edit comment</t>
   </si>
   <si>
@@ -343,6 +325,21 @@
   </si>
   <si>
     <t>endpoints to handle ratings</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>places/search?c=&amp;k=</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,12 +445,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -510,9 +501,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -561,10 +552,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -572,16 +562,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -876,8 +866,8 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -900,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
@@ -926,7 +916,7 @@
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -940,22 +930,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3">
         <v>201</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="38"/>
+        <v>11</v>
+      </c>
+      <c r="H4" s="37"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -964,15 +954,15 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3">
         <v>302</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="41"/>
+        <v>12</v>
+      </c>
+      <c r="H5" s="40"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -981,11 +971,11 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="38"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -994,11 +984,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="38"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1009,30 +999,30 @@
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="38"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="3">
         <v>200</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="38"/>
+        <v>14</v>
+      </c>
+      <c r="H9" s="37"/>
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1041,15 +1031,15 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3">
         <v>406</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="38"/>
+        <v>17</v>
+      </c>
+      <c r="H10" s="37"/>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1060,30 +1050,30 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="3">
         <v>200</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="42"/>
+        <v>14</v>
+      </c>
+      <c r="H12" s="41"/>
       <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1092,15 +1082,15 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
         <v>404</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="H13" s="37"/>
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1113,9 +1103,9 @@
         <v>403</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="38"/>
+        <v>90</v>
+      </c>
+      <c r="H14" s="37"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1128,9 +1118,9 @@
         <v>406</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" s="38"/>
+        <v>76</v>
+      </c>
+      <c r="H15" s="37"/>
       <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1141,30 +1131,30 @@
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="38"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="3">
         <v>200</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="38"/>
+        <v>20</v>
+      </c>
+      <c r="H17" s="37"/>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1177,9 +1167,9 @@
         <v>404</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="H18" s="37"/>
       <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1190,64 +1180,64 @@
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="38"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="3">
         <v>200</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="42"/>
+        <v>22</v>
+      </c>
+      <c r="H20" s="41"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="36">
+        <v>404</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="37"/>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="36">
+        <v>406</v>
+      </c>
+      <c r="G22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="37">
-        <v>404</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="37">
-        <v>406</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="38"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1263,7 +1253,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1276,27 +1266,27 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F25" s="9">
         <v>201</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="39"/>
+        <v>25</v>
+      </c>
+      <c r="H25" s="38"/>
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1305,11 +1295,11 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="39"/>
+      <c r="H26" s="38"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1318,11 +1308,11 @@
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="39"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1331,11 +1321,11 @@
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="39"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1344,11 +1334,11 @@
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="39"/>
+      <c r="H29" s="38"/>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1359,30 +1349,30 @@
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
       <c r="G30" s="11"/>
-      <c r="H30" s="40"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="9">
         <v>200</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="40"/>
+        <v>25</v>
+      </c>
+      <c r="H31" s="39"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1393,9 +1383,9 @@
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="G32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="40"/>
+        <v>26</v>
+      </c>
+      <c r="H32" s="39"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1406,9 +1396,9 @@
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
       <c r="G33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="40"/>
+        <v>27</v>
+      </c>
+      <c r="H33" s="39"/>
       <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1419,9 +1409,9 @@
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
       <c r="G34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="40"/>
+        <v>28</v>
+      </c>
+      <c r="H34" s="39"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1432,32 +1422,30 @@
       <c r="E35" s="11"/>
       <c r="F35" s="12"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="40"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>33</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E36" s="8"/>
       <c r="F36" s="9">
         <v>200</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="40"/>
+        <v>25</v>
+      </c>
+      <c r="H36" s="39"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1465,14 +1453,12 @@
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="E37" s="8"/>
       <c r="F37" s="9"/>
       <c r="G37" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="40"/>
+        <v>26</v>
+      </c>
+      <c r="H37" s="39"/>
       <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1483,9 +1469,9 @@
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
       <c r="G38" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="40"/>
+        <v>27</v>
+      </c>
+      <c r="H38" s="39"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1496,9 +1482,9 @@
       <c r="E39" s="8"/>
       <c r="F39" s="9"/>
       <c r="G39" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="40"/>
+        <v>28</v>
+      </c>
+      <c r="H39" s="39"/>
       <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1514,25 +1500,25 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="9">
         <v>200</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="35"/>
+        <v>25</v>
+      </c>
+      <c r="H41" s="34"/>
       <c r="I41" s="17"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1543,9 +1529,9 @@
       <c r="E42" s="8"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H42" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="H42" s="34"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -1556,9 +1542,9 @@
       <c r="E43" s="8"/>
       <c r="F43" s="9"/>
       <c r="G43" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="35"/>
+        <v>28</v>
+      </c>
+      <c r="H43" s="34"/>
       <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1569,9 +1555,9 @@
       <c r="E44" s="8"/>
       <c r="F44" s="9"/>
       <c r="G44" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H44" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="H44" s="34"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -1582,30 +1568,30 @@
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
       <c r="G45" s="11"/>
-      <c r="H45" s="35"/>
+      <c r="H45" s="34"/>
       <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>25</v>
+        <v>81</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="27">
         <v>200</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H46" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="H46" s="34"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -1616,32 +1602,32 @@
       <c r="E47" s="11"/>
       <c r="F47" s="12"/>
       <c r="G47" s="11"/>
-      <c r="H47" s="35"/>
+      <c r="H47" s="34"/>
       <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F48" s="27">
         <v>201</v>
       </c>
       <c r="G48" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="H48" s="35"/>
+        <v>83</v>
+      </c>
+      <c r="H48" s="34"/>
       <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -1652,30 +1638,30 @@
       <c r="E49" s="11"/>
       <c r="F49" s="12"/>
       <c r="G49" s="11"/>
-      <c r="H49" s="35"/>
+      <c r="H49" s="34"/>
       <c r="I49" s="17"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="9">
         <v>200</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H50" s="35"/>
+        <v>85</v>
+      </c>
+      <c r="H50" s="34"/>
       <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -1686,9 +1672,9 @@
       <c r="E51" s="8"/>
       <c r="F51" s="9"/>
       <c r="G51" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H51" s="35"/>
+        <v>86</v>
+      </c>
+      <c r="H51" s="34"/>
       <c r="I51" s="17"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -1699,9 +1685,9 @@
       <c r="E52" s="8"/>
       <c r="F52" s="9"/>
       <c r="G52" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H52" s="35"/>
+        <v>87</v>
+      </c>
+      <c r="H52" s="34"/>
       <c r="I52" s="17"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -1712,30 +1698,30 @@
       <c r="E53" s="11"/>
       <c r="F53" s="12"/>
       <c r="G53" s="11"/>
-      <c r="H53" s="35"/>
+      <c r="H53" s="34"/>
       <c r="I53" s="17"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="9">
         <v>200</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H54" s="35"/>
+        <v>25</v>
+      </c>
+      <c r="H54" s="34"/>
       <c r="I54" s="17"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -1746,9 +1732,9 @@
       <c r="E55" s="8"/>
       <c r="F55" s="9"/>
       <c r="G55" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H55" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="H55" s="34"/>
       <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -1759,9 +1745,9 @@
       <c r="E56" s="8"/>
       <c r="F56" s="9"/>
       <c r="G56" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H56" s="35"/>
+        <v>27</v>
+      </c>
+      <c r="H56" s="34"/>
       <c r="I56" s="17"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -1772,9 +1758,9 @@
       <c r="E57" s="8"/>
       <c r="F57" s="9"/>
       <c r="G57" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H57" s="35"/>
+        <v>28</v>
+      </c>
+      <c r="H57" s="34"/>
       <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -1785,32 +1771,32 @@
       <c r="E58" s="11"/>
       <c r="F58" s="12"/>
       <c r="G58" s="11"/>
-      <c r="H58" s="35"/>
+      <c r="H58" s="34"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F59" s="9">
         <v>201</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H59" s="35"/>
+        <v>46</v>
+      </c>
+      <c r="H59" s="34"/>
       <c r="I59" s="17"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -1821,30 +1807,30 @@
       <c r="E60" s="11"/>
       <c r="F60" s="12"/>
       <c r="G60" s="11"/>
-      <c r="H60" s="35"/>
+      <c r="H60" s="34"/>
       <c r="I60" s="17"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="9">
         <v>200</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H61" s="35"/>
+        <v>48</v>
+      </c>
+      <c r="H61" s="34"/>
       <c r="I61" s="17"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -1855,30 +1841,30 @@
       <c r="E62" s="11"/>
       <c r="F62" s="12"/>
       <c r="G62" s="11"/>
-      <c r="H62" s="35"/>
+      <c r="H62" s="34"/>
       <c r="I62" s="17"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="9">
         <v>200</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H63" s="35"/>
+        <v>25</v>
+      </c>
+      <c r="H63" s="34"/>
       <c r="I63" s="17"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -1889,9 +1875,9 @@
       <c r="E64" s="8"/>
       <c r="F64" s="9"/>
       <c r="G64" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H64" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="H64" s="34"/>
       <c r="I64" s="17"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -1902,9 +1888,9 @@
       <c r="E65" s="8"/>
       <c r="F65" s="9"/>
       <c r="G65" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H65" s="35"/>
+        <v>27</v>
+      </c>
+      <c r="H65" s="34"/>
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -1915,9 +1901,9 @@
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>
       <c r="G66" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H66" s="35"/>
+        <v>28</v>
+      </c>
+      <c r="H66" s="34"/>
       <c r="I66" s="17"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -1928,32 +1914,32 @@
       <c r="E67" s="11"/>
       <c r="F67" s="12"/>
       <c r="G67" s="11"/>
-      <c r="H67" s="35"/>
+      <c r="H67" s="34"/>
       <c r="I67" s="17"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F68" s="9">
         <v>201</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H68" s="35"/>
+        <v>46</v>
+      </c>
+      <c r="H68" s="34"/>
       <c r="I68" s="17"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -1964,30 +1950,30 @@
       <c r="E69" s="11"/>
       <c r="F69" s="12"/>
       <c r="G69" s="11"/>
-      <c r="H69" s="35"/>
+      <c r="H69" s="34"/>
       <c r="I69" s="17"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="9">
         <v>200</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H70" s="35"/>
+        <v>48</v>
+      </c>
+      <c r="H70" s="34"/>
       <c r="I70" s="17"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -1998,12 +1984,12 @@
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
       <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
+      <c r="H71" s="34"/>
       <c r="I71" s="17"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -2011,224 +1997,224 @@
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
+      <c r="H72" s="34"/>
       <c r="I72" s="17"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B73" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="30" t="s">
+      <c r="A73" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F73" s="30">
+        <v>201</v>
+      </c>
+      <c r="G73" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73" s="34"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="28"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F74" s="30"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="31"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="34"/>
+      <c r="I75" s="17"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F76" s="30">
+        <v>200</v>
+      </c>
+      <c r="G76" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H76" s="34"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="31"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="34"/>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C78" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D73" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F73" s="31">
+      <c r="D78" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="30">
+        <v>200</v>
+      </c>
+      <c r="G78" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H78" s="34"/>
+      <c r="I78" s="17"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="31"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="17"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="17"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F81" s="30">
         <v>201</v>
       </c>
-      <c r="G73" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="17"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="29"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F74" s="31"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="17"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="32"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="17"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B76" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D76" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F76" s="31">
+      <c r="G81" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H81" s="34"/>
+      <c r="I81" s="17"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="28"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F82" s="30"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="34"/>
+      <c r="I82" s="17"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="31"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="34"/>
+      <c r="I83" s="17"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F84" s="30">
         <v>200</v>
       </c>
-      <c r="G76" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H76" s="28"/>
-      <c r="I76" s="17"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="32"/>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="33"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="17"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B78" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E78" s="30"/>
-      <c r="F78" s="31">
-        <v>200</v>
-      </c>
-      <c r="G78" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H78" s="28"/>
-      <c r="I78" s="17"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="32"/>
-      <c r="B79" s="33"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="17"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="33"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="17"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D81" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F81" s="31">
-        <v>201</v>
-      </c>
-      <c r="G81" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H81" s="28"/>
-      <c r="I81" s="17"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="29"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F82" s="31"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="28"/>
-      <c r="I82" s="17"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="32"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="33"/>
-      <c r="H83" s="28"/>
-      <c r="I83" s="17"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C84" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="D84" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F84" s="31">
-        <v>200</v>
-      </c>
-      <c r="G84" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H84" s="28"/>
+      <c r="G84" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H84" s="34"/>
       <c r="I84" s="17"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="32"/>
-      <c r="B85" s="33"/>
-      <c r="C85" s="33"/>
-      <c r="D85" s="33"/>
-      <c r="E85" s="33"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="33"/>
-      <c r="H85" s="28"/>
+      <c r="A85" s="31"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="34"/>
       <c r="I85" s="17"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -2239,12 +2225,12 @@
       <c r="E86" s="14"/>
       <c r="F86" s="15"/>
       <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
+      <c r="H86" s="34"/>
       <c r="I86" s="17"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -2252,30 +2238,30 @@
       <c r="E87" s="14"/>
       <c r="F87" s="15"/>
       <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
+      <c r="H87" s="34"/>
       <c r="I87" s="17"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E88" s="18"/>
       <c r="F88" s="19">
         <v>200</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H88" s="35"/>
+        <v>67</v>
+      </c>
+      <c r="H88" s="34"/>
       <c r="I88" s="17"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -2286,9 +2272,9 @@
       <c r="E89" s="18"/>
       <c r="F89" s="19"/>
       <c r="G89" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H89" s="35"/>
+        <v>68</v>
+      </c>
+      <c r="H89" s="34"/>
       <c r="I89" s="17"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -2299,9 +2285,9 @@
       <c r="E90" s="18"/>
       <c r="F90" s="19"/>
       <c r="G90" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="35"/>
+        <v>9</v>
+      </c>
+      <c r="H90" s="34"/>
       <c r="I90" s="17"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
@@ -2312,9 +2298,9 @@
       <c r="E91" s="18"/>
       <c r="F91" s="19"/>
       <c r="G91" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H91" s="35"/>
+        <v>27</v>
+      </c>
+      <c r="H91" s="34"/>
       <c r="I91" s="17"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -2325,32 +2311,32 @@
       <c r="E92" s="20"/>
       <c r="F92" s="21"/>
       <c r="G92" s="20"/>
-      <c r="H92" s="35"/>
+      <c r="H92" s="34"/>
       <c r="I92" s="17"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="18" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F93" s="19">
         <v>200</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H93" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="H93" s="34"/>
       <c r="I93" s="17"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -2359,11 +2345,11 @@
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="18" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F94" s="19"/>
       <c r="G94" s="18"/>
-      <c r="H94" s="35"/>
+      <c r="H94" s="34"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
@@ -2373,31 +2359,31 @@
       <c r="E95" s="20"/>
       <c r="F95" s="21"/>
       <c r="G95" s="20"/>
-      <c r="H95" s="35"/>
+      <c r="H95" s="34"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F96" s="19">
         <v>200</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H96" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="H96" s="34"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="20"/>
@@ -2407,31 +2393,31 @@
       <c r="E97" s="20"/>
       <c r="F97" s="21"/>
       <c r="G97" s="20"/>
-      <c r="H97" s="35"/>
+      <c r="H97" s="34"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F98" s="19">
         <v>200</v>
       </c>
       <c r="G98" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H98" s="42"/>
+        <v>22</v>
+      </c>
+      <c r="H98" s="41"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="18"/>
@@ -2439,15 +2425,15 @@
       <c r="C99" s="18"/>
       <c r="D99" s="18"/>
       <c r="E99" s="18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F99" s="19">
         <v>406</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H99" s="35"/>
+        <v>76</v>
+      </c>
+      <c r="H99" s="34"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="14"/>
@@ -2460,7 +2446,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B101" s="14"/>
       <c r="C101" s="14"/>
@@ -2471,27 +2457,27 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F102" s="16">
         <v>200</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H102" s="40"/>
+        <v>88</v>
+      </c>
+      <c r="H102" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
making improvements and fixing bugs
</commit_message>
<xml_diff>
--- a/endpoints.xlsx
+++ b/endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Grad Proj\grad-proj-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBBD655-CB88-4C75-A139-65E18B1E89AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DF04F1-E6E4-474A-BA25-D5EEC31D360D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="endpoints" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
   <si>
     <t>route</t>
   </si>
@@ -96,9 +96,6 @@
     <t>changed</t>
   </si>
   <si>
-    <t>places/rec</t>
-  </si>
-  <si>
     <t>Authorization</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>places/&lt;id&gt;/comments/&lt;p&gt;</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -340,6 +334,27 @@
   </si>
   <si>
     <t>places/search?c=&amp;k=</t>
+  </si>
+  <si>
+    <t>auth/refresh_token</t>
+  </si>
+  <si>
+    <t>get new web token</t>
+  </si>
+  <si>
+    <t>old_token</t>
+  </si>
+  <si>
+    <t>refresh_token</t>
+  </si>
+  <si>
+    <t>expired or invalid</t>
+  </si>
+  <si>
+    <t>places/&lt;id&gt;/comments?page</t>
+  </si>
+  <si>
+    <t>places/rec?page</t>
   </si>
 </sst>
 </file>
@@ -503,7 +518,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -572,6 +587,10 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -863,11 +882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D813DE80-0DAC-45D8-A4FE-65EF077BEFD0}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -890,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
@@ -916,7 +935,7 @@
     </row>
     <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -930,10 +949,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
@@ -1007,10 +1026,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
@@ -1058,10 +1077,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
@@ -1103,7 +1122,7 @@
         <v>403</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H14" s="37"/>
       <c r="I14" s="17"/>
@@ -1118,7 +1137,7 @@
         <v>406</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H15" s="37"/>
       <c r="I15" s="17"/>
@@ -1139,10 +1158,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
@@ -1188,10 +1207,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
@@ -1240,91 +1259,102 @@
       <c r="H22" s="37"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="17"/>
+      <c r="A24" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="36">
+        <v>403</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="37"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="36">
+        <v>200</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="37"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="9">
+        <v>201</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="9">
-        <v>201</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="38"/>
-      <c r="I25" s="17"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
       <c r="H28" s="38"/>
       <c r="I28" s="17"/>
     </row>
@@ -1334,7 +1364,7 @@
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="8"/>
@@ -1342,37 +1372,29 @@
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="39"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9">
-        <v>200</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="39"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="38"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1380,70 +1402,70 @@
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="F32" s="9"/>
-      <c r="G32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H32" s="39"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="38"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="39"/>
       <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="A34" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
+      <c r="F34" s="9">
+        <v>200</v>
+      </c>
       <c r="G34" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H34" s="39"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="11"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H35" s="39"/>
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="9">
-        <v>200</v>
-      </c>
+      <c r="F36" s="9"/>
       <c r="G36" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H36" s="39"/>
       <c r="I36" s="17"/>
@@ -1456,69 +1478,69 @@
       <c r="E37" s="8"/>
       <c r="F37" s="9"/>
       <c r="G37" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H37" s="39"/>
       <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="11"/>
       <c r="H38" s="39"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="A39" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
+      <c r="F39" s="9">
+        <v>200</v>
+      </c>
       <c r="G39" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H39" s="39"/>
       <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="17"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="39"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="9">
-        <v>200</v>
-      </c>
+      <c r="F41" s="9"/>
       <c r="G41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="34"/>
+        <v>26</v>
+      </c>
+      <c r="H41" s="39"/>
       <c r="I41" s="17"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1529,197 +1551,197 @@
       <c r="E42" s="8"/>
       <c r="F42" s="9"/>
       <c r="G42" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" s="34"/>
+        <v>27</v>
+      </c>
+      <c r="H42" s="39"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H43" s="34"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="17"/>
       <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
+      <c r="A44" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
+      <c r="F44" s="9">
+        <v>200</v>
+      </c>
       <c r="G44" s="8" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="11"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H45" s="34"/>
       <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27">
-        <v>200</v>
-      </c>
-      <c r="G46" s="26" t="s">
-        <v>26</v>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="H46" s="34"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="11"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="H47" s="34"/>
       <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="27">
-        <v>201</v>
-      </c>
-      <c r="G48" s="26" t="s">
-        <v>83</v>
-      </c>
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="11"/>
       <c r="H48" s="34"/>
       <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="11"/>
+      <c r="A49" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27">
+        <v>200</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="H49" s="34"/>
       <c r="I49" s="17"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="9">
-        <v>200</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="11"/>
       <c r="H50" s="34"/>
       <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="8" t="s">
-        <v>86</v>
+      <c r="A51" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="27">
+        <v>201</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="H51" s="34"/>
       <c r="I51" s="17"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="8" t="s">
-        <v>87</v>
-      </c>
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="11"/>
       <c r="H52" s="34"/>
       <c r="I52" s="17"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="11"/>
+      <c r="A53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="9">
+        <v>200</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="H53" s="34"/>
       <c r="I53" s="17"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="F54" s="9">
-        <v>200</v>
-      </c>
+      <c r="F54" s="9"/>
       <c r="G54" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="H54" s="34"/>
       <c r="I54" s="17"/>
@@ -1732,397 +1754,397 @@
       <c r="E55" s="8"/>
       <c r="F55" s="9"/>
       <c r="G55" s="8" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="H55" s="34"/>
       <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="11"/>
       <c r="H56" s="34"/>
       <c r="I56" s="17"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="A57" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E57" s="8"/>
-      <c r="F57" s="9"/>
+      <c r="F57" s="9">
+        <v>200</v>
+      </c>
       <c r="G57" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H57" s="34"/>
       <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="11"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H58" s="34"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="9">
-        <v>201</v>
-      </c>
+      <c r="A59" s="7"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="9"/>
       <c r="G59" s="8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="H59" s="34"/>
       <c r="I59" s="17"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="11"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="H60" s="34"/>
       <c r="I60" s="17"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="9">
-        <v>200</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A61" s="10"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="11"/>
       <c r="H61" s="34"/>
       <c r="I61" s="17"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="11"/>
+      <c r="A62" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="9">
+        <v>201</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="H62" s="34"/>
       <c r="I62" s="17"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="9">
-        <v>200</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="11"/>
       <c r="H63" s="34"/>
       <c r="I63" s="17"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="7"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
+      <c r="A64" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E64" s="8"/>
-      <c r="F64" s="9"/>
+      <c r="F64" s="9">
+        <v>200</v>
+      </c>
       <c r="G64" s="8" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="H64" s="34"/>
       <c r="I64" s="17"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="11"/>
       <c r="H65" s="34"/>
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
+      <c r="A66" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="E66" s="8"/>
-      <c r="F66" s="9"/>
+      <c r="F66" s="9">
+        <v>200</v>
+      </c>
       <c r="G66" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H66" s="34"/>
       <c r="I66" s="17"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="10"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="11"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H67" s="34"/>
       <c r="I67" s="17"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F68" s="9">
-        <v>201</v>
-      </c>
+      <c r="A68" s="7"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="9"/>
       <c r="G68" s="8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="H68" s="34"/>
       <c r="I68" s="17"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="11"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="H69" s="34"/>
       <c r="I69" s="17"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="9">
-        <v>200</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="11"/>
       <c r="H70" s="34"/>
       <c r="I70" s="17"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
+      <c r="A71" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F71" s="9">
+        <v>201</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="H71" s="34"/>
       <c r="I71" s="17"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="11"/>
       <c r="H72" s="34"/>
       <c r="I72" s="17"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" s="29" t="s">
+      <c r="A73" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C73" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E73" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F73" s="30">
-        <v>201</v>
-      </c>
-      <c r="G73" s="29" t="s">
-        <v>25</v>
+      <c r="C73" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="9">
+        <v>200</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="17"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="28"/>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F74" s="30"/>
-      <c r="G74" s="29"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
       <c r="H74" s="34"/>
       <c r="I74" s="17"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="31"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="32"/>
+      <c r="A75" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
       <c r="H75" s="34"/>
       <c r="I75" s="17"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="28" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B76" s="29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D76" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F76" s="30">
+        <v>201</v>
+      </c>
+      <c r="G76" s="29" t="s">
         <v>24</v>
-      </c>
-      <c r="E76" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F76" s="30">
-        <v>200</v>
-      </c>
-      <c r="G76" s="29" t="s">
-        <v>25</v>
       </c>
       <c r="H76" s="34"/>
       <c r="I76" s="17"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="31"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="32"/>
+      <c r="A77" s="28"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F77" s="30"/>
+      <c r="G77" s="29"/>
       <c r="H77" s="34"/>
       <c r="I77" s="17"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C78" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D78" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="30">
-        <v>200</v>
-      </c>
-      <c r="G78" s="29" t="s">
-        <v>48</v>
-      </c>
+      <c r="A78" s="31"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="32"/>
       <c r="H78" s="34"/>
       <c r="I78" s="17"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="31"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="32"/>
+      <c r="A79" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F79" s="30">
+        <v>200</v>
+      </c>
+      <c r="G79" s="29" t="s">
+        <v>24</v>
+      </c>
       <c r="H79" s="34"/>
       <c r="I79" s="17"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="31" t="s">
-        <v>99</v>
-      </c>
+      <c r="A80" s="31"/>
       <c r="B80" s="32"/>
       <c r="C80" s="32"/>
       <c r="D80" s="32"/>
@@ -2134,44 +2156,42 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="28" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="B81" s="29" t="s">
         <v>100</v>
       </c>
       <c r="C81" s="29" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81" s="29" t="s">
-        <v>56</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E81" s="29"/>
       <c r="F81" s="30">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G81" s="29" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H81" s="34"/>
       <c r="I81" s="17"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="28"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F82" s="30"/>
-      <c r="G82" s="29"/>
+      <c r="A82" s="31"/>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="32"/>
       <c r="H82" s="34"/>
       <c r="I82" s="17"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="31"/>
+      <c r="A83" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="B83" s="32"/>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
@@ -2183,158 +2203,158 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="29" t="s">
-        <v>103</v>
-      </c>
       <c r="C84" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D84" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84" s="30">
+        <v>201</v>
+      </c>
+      <c r="G84" s="29" t="s">
         <v>24</v>
-      </c>
-      <c r="E84" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F84" s="30">
-        <v>200</v>
-      </c>
-      <c r="G84" s="29" t="s">
-        <v>25</v>
       </c>
       <c r="H84" s="34"/>
       <c r="I84" s="17"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="31"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="33"/>
-      <c r="G85" s="32"/>
+      <c r="A85" s="28"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F85" s="30"/>
+      <c r="G85" s="29"/>
       <c r="H85" s="34"/>
       <c r="I85" s="17"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="14"/>
+      <c r="A86" s="31"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="32"/>
       <c r="H86" s="34"/>
       <c r="I86" s="17"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="14"/>
+      <c r="A87" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F87" s="30">
+        <v>200</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>24</v>
+      </c>
       <c r="H87" s="34"/>
       <c r="I87" s="17"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C88" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E88" s="18"/>
-      <c r="F88" s="19">
-        <v>200</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>67</v>
-      </c>
+      <c r="A88" s="31"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="32"/>
       <c r="H88" s="34"/>
       <c r="I88" s="17"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="18"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="18" t="s">
-        <v>68</v>
-      </c>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="14"/>
       <c r="H89" s="34"/>
       <c r="I89" s="17"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="18"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="A90" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="14"/>
       <c r="H90" s="34"/>
       <c r="I90" s="17"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="18"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
+      <c r="A91" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="E91" s="18"/>
-      <c r="F91" s="19"/>
+      <c r="F91" s="19">
+        <v>200</v>
+      </c>
       <c r="G91" s="18" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="H91" s="34"/>
       <c r="I91" s="17"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="20"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="H92" s="34"/>
       <c r="I92" s="17"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D93" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F93" s="19">
-        <v>200</v>
-      </c>
+      <c r="A93" s="18"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="19"/>
       <c r="G93" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="H93" s="34"/>
       <c r="I93" s="17"/>
@@ -2344,12 +2364,13 @@
       <c r="B94" s="18"/>
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
-      <c r="E94" s="18" t="s">
-        <v>68</v>
-      </c>
+      <c r="E94" s="18"/>
       <c r="F94" s="19"/>
-      <c r="G94" s="18"/>
+      <c r="G94" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="H94" s="34"/>
+      <c r="I94" s="17"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
@@ -2360,22 +2381,23 @@
       <c r="F95" s="21"/>
       <c r="G95" s="20"/>
       <c r="H95" s="34"/>
+      <c r="I95" s="17"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F96" s="19">
         <v>200</v>
@@ -2384,100 +2406,147 @@
         <v>22</v>
       </c>
       <c r="H96" s="34"/>
+      <c r="I96" s="17"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="20"/>
+      <c r="A97" s="18"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F97" s="19"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="34"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="18" t="s">
+      <c r="A98" s="20"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="34"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F99" s="19">
+        <v>200</v>
+      </c>
+      <c r="G99" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H99" s="34"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="20"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="34"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E101" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B98" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C98" s="18" t="s">
+      <c r="F101" s="19">
+        <v>200</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H101" s="41"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D98" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E98" s="18" t="s">
+      <c r="F102" s="19">
+        <v>406</v>
+      </c>
+      <c r="G102" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F98" s="19">
+      <c r="H102" s="34"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="14"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="14"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F105" s="16">
         <v>200</v>
       </c>
-      <c r="G98" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H98" s="41"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="18"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F99" s="19">
-        <v>406</v>
-      </c>
-      <c r="G99" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H99" s="34"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="14"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="14"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F102" s="16">
-        <v>200</v>
-      </c>
-      <c r="G102" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H102" s="39"/>
+      <c r="G105" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H105" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>